<commit_message>
Ignore large fasta files
</commit_message>
<xml_diff>
--- a/00-Phylogenetics/Resources/03-Dong2022/List_of_Dong42.xlsx
+++ b/00-Phylogenetics/Resources/03-Dong2022/List_of_Dong42.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunrui/Library/CloudStorage/OneDrive-Personal/Marchantia/Codes_Analysis/Phylogenetics/00-Dong42/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunrui/Library/CloudStorage/OneDrive-Personal/Marchantia/Codes_Analysis/Phylogenetics/Resources/03-Dong2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC64E63C-D7B5-0342-BE6D-B48F1C28E26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B6A2F4-0521-2946-805D-47331CE5E476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9720" yWindow="960" windowWidth="37060" windowHeight="21100" xr2:uid="{6AEF4972-0A12-934A-ACAB-8A36349463F1}"/>
+    <workbookView xWindow="1440" yWindow="500" windowWidth="36960" windowHeight="21100" xr2:uid="{6AEF4972-0A12-934A-ACAB-8A36349463F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="372">
   <si>
     <t>Order</t>
   </si>
@@ -1112,6 +1112,174 @@
   </si>
   <si>
     <t>Mpolymorpha.pep</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Dong_Hmnioides</t>
+  </si>
+  <si>
+    <t>Dong_Tlacunosa</t>
+  </si>
+  <si>
+    <t>Dong_Apinguis</t>
+  </si>
+  <si>
+    <t>Dong_Asharpii</t>
+  </si>
+  <si>
+    <t>Dong_Bbarbata</t>
+  </si>
+  <si>
+    <t>Dong_Bjaponica</t>
+  </si>
+  <si>
+    <t>Dong_Btrilobata</t>
+  </si>
+  <si>
+    <t>Dong_Cfissa</t>
+  </si>
+  <si>
+    <t>Dong_Fcristula</t>
+  </si>
+  <si>
+    <t>Dong_Forientalis</t>
+  </si>
+  <si>
+    <t>Dong_Frullania</t>
+  </si>
+  <si>
+    <t>Dong_Hdicranus</t>
+  </si>
+  <si>
+    <t>Dong_Hramosus</t>
+  </si>
+  <si>
+    <t>Dong_Hzollingeri</t>
+  </si>
+  <si>
+    <t>Dong_Lsandvicensis</t>
+  </si>
+  <si>
+    <t>Dong_Ltrichodes</t>
+  </si>
+  <si>
+    <t>Dong_Mcrispata</t>
+  </si>
+  <si>
+    <t>Dong_Malternifolia</t>
+  </si>
+  <si>
+    <t>Dong_Mcrassipilis</t>
+  </si>
+  <si>
+    <t>Dong_Mleptoneura</t>
+  </si>
+  <si>
+    <t>Dong_Mnuda</t>
+  </si>
+  <si>
+    <t>Dong_Ncurvifolia</t>
+  </si>
+  <si>
+    <t>Dong_Ogrosseverrucosum</t>
+  </si>
+  <si>
+    <t>Dong_Oprostratum</t>
+  </si>
+  <si>
+    <t>Dong_Plyellii</t>
+  </si>
+  <si>
+    <t>Dong_Pendiviifolia</t>
+  </si>
+  <si>
+    <t>Dong_Pasplenioides</t>
+  </si>
+  <si>
+    <t>Dong_Psubtropica</t>
+  </si>
+  <si>
+    <t>Dong_Ppurpurea</t>
+  </si>
+  <si>
+    <t>Dong_Phirtellus</t>
+  </si>
+  <si>
+    <t>Dong_Pnavicularis</t>
+  </si>
+  <si>
+    <t>Dong_Ppinnata</t>
+  </si>
+  <si>
+    <t>Dong_Pplumosa</t>
+  </si>
+  <si>
+    <t>Dong_Ppulcherrimum</t>
+  </si>
+  <si>
+    <t>Dong_Pstriatus</t>
+  </si>
+  <si>
+    <t>Dong_Rjaponica</t>
+  </si>
+  <si>
+    <t>Dong_Rlindenbergia</t>
+  </si>
+  <si>
+    <t>Dong_Rlatifrons</t>
+  </si>
+  <si>
+    <t>Dong_Snemorosa</t>
+  </si>
+  <si>
+    <t>Dong_Sornithopodioides</t>
+  </si>
+  <si>
+    <t>Dong_Schistochila</t>
+  </si>
+  <si>
+    <t>Dong_Ttomentella</t>
+  </si>
+  <si>
+    <t>Dong_Awallichiana</t>
+  </si>
+  <si>
+    <t>Dong_Bpusilla</t>
+  </si>
+  <si>
+    <t>Dong_Cconicum</t>
+  </si>
+  <si>
+    <t>Dong_Dhirsuta</t>
+  </si>
+  <si>
+    <t>Dong_Lcruciata</t>
+  </si>
+  <si>
+    <t>Dong_Mpaleacea</t>
+  </si>
+  <si>
+    <t>Dong_Mpolymorpha</t>
+  </si>
+  <si>
+    <t>Dong_Mtenerum</t>
+  </si>
+  <si>
+    <t>Dong_Rberychiana</t>
+  </si>
+  <si>
+    <t>Dong_Rcavernosa</t>
+  </si>
+  <si>
+    <t>Dong_Stexanus</t>
+  </si>
+  <si>
+    <t>Dong_Wdenudata</t>
+  </si>
+  <si>
+    <t>Dong_Pepiphylla</t>
   </si>
 </sst>
 </file>
@@ -1592,10 +1760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB154F9F-AECA-5E46-A1E9-CB02F56C7F51}">
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1605,9 +1773,10 @@
     <col min="3" max="6" width="10.83203125" customWidth="1"/>
     <col min="7" max="7" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>80</v>
       </c>
@@ -1635,8 +1804,11 @@
       <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>309</v>
       </c>
@@ -1660,7 +1832,7 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>303</v>
       </c>
@@ -1684,7 +1856,7 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>90</v>
       </c>
@@ -1712,8 +1884,11 @@
       <c r="I4" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>85</v>
       </c>
@@ -1741,8 +1916,11 @@
       <c r="I5" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>164</v>
       </c>
@@ -1770,8 +1948,11 @@
       <c r="I6" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>168</v>
       </c>
@@ -1799,8 +1980,11 @@
       <c r="I7" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>230</v>
       </c>
@@ -1828,8 +2012,11 @@
       <c r="I8" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>235</v>
       </c>
@@ -1857,8 +2044,11 @@
       <c r="I9" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>239</v>
       </c>
@@ -1886,8 +2076,11 @@
       <c r="I10" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>242</v>
       </c>
@@ -1915,8 +2108,11 @@
       <c r="I11" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>160</v>
       </c>
@@ -1944,8 +2140,11 @@
       <c r="I12" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>190</v>
       </c>
@@ -1973,8 +2172,11 @@
       <c r="I13" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>195</v>
       </c>
@@ -2002,8 +2204,11 @@
       <c r="I14" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>246</v>
       </c>
@@ -2031,8 +2236,11 @@
       <c r="I15" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>250</v>
       </c>
@@ -2060,8 +2268,11 @@
       <c r="I16" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>253</v>
       </c>
@@ -2089,8 +2300,11 @@
       <c r="I17" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>257</v>
       </c>
@@ -2118,8 +2332,11 @@
       <c r="I18" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>260</v>
       </c>
@@ -2147,8 +2364,11 @@
       <c r="I19" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>171</v>
       </c>
@@ -2176,8 +2396,11 @@
       <c r="I20" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>263</v>
       </c>
@@ -2205,8 +2428,11 @@
       <c r="I21" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>175</v>
       </c>
@@ -2234,8 +2460,11 @@
       <c r="I22" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>179</v>
       </c>
@@ -2263,8 +2492,11 @@
       <c r="I23" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>267</v>
       </c>
@@ -2292,8 +2524,11 @@
       <c r="I24" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>270</v>
       </c>
@@ -2321,8 +2556,11 @@
       <c r="I25" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>274</v>
       </c>
@@ -2350,8 +2588,11 @@
       <c r="I26" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>277</v>
       </c>
@@ -2379,8 +2620,11 @@
       <c r="I27" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>156</v>
       </c>
@@ -2408,8 +2652,11 @@
       <c r="I28" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>148</v>
       </c>
@@ -2437,8 +2684,11 @@
       <c r="I29" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>153</v>
       </c>
@@ -2466,8 +2716,11 @@
       <c r="I30" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>280</v>
       </c>
@@ -2495,8 +2748,11 @@
       <c r="I31" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J31" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>284</v>
       </c>
@@ -2524,8 +2780,11 @@
       <c r="I32" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>186</v>
       </c>
@@ -2553,8 +2812,11 @@
       <c r="I33" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>287</v>
       </c>
@@ -2582,8 +2844,11 @@
       <c r="I34" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J34" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>198</v>
       </c>
@@ -2611,8 +2876,11 @@
       <c r="I35" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>203</v>
       </c>
@@ -2640,8 +2908,11 @@
       <c r="I36" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J36" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>206</v>
       </c>
@@ -2669,8 +2940,11 @@
       <c r="I37" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J37" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>221</v>
       </c>
@@ -2698,8 +2972,11 @@
       <c r="I38" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J38" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>209</v>
       </c>
@@ -2727,8 +3004,11 @@
       <c r="I39" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J39" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>213</v>
       </c>
@@ -2756,8 +3036,11 @@
       <c r="I40" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J40" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>217</v>
       </c>
@@ -2785,8 +3068,11 @@
       <c r="I41" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J41" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>183</v>
       </c>
@@ -2814,8 +3100,11 @@
       <c r="I42" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J42" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>291</v>
       </c>
@@ -2843,8 +3132,11 @@
       <c r="I43" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J43" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>296</v>
       </c>
@@ -2872,8 +3164,11 @@
       <c r="I44" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J44" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>225</v>
       </c>
@@ -2901,8 +3196,11 @@
       <c r="I45" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J45" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>299</v>
       </c>
@@ -2930,8 +3228,11 @@
       <c r="I46" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J46" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>110</v>
       </c>
@@ -2959,8 +3260,11 @@
       <c r="I47" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>94</v>
       </c>
@@ -2988,8 +3292,11 @@
       <c r="I48" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J48" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>115</v>
       </c>
@@ -3017,8 +3324,11 @@
       <c r="I49" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J49" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>119</v>
       </c>
@@ -3046,8 +3356,11 @@
       <c r="I50" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J50" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>105</v>
       </c>
@@ -3075,8 +3388,11 @@
       <c r="I51" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J51" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>123</v>
       </c>
@@ -3104,8 +3420,11 @@
       <c r="I52" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J52" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
         <v>129</v>
       </c>
@@ -3133,8 +3452,11 @@
       <c r="I53" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J53" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>133</v>
       </c>
@@ -3162,8 +3484,11 @@
       <c r="I54" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J54" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
         <v>137</v>
       </c>
@@ -3191,8 +3516,11 @@
       <c r="I55" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J55" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>141</v>
       </c>
@@ -3220,8 +3548,11 @@
       <c r="I56" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J56" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>99</v>
       </c>
@@ -3249,8 +3580,11 @@
       <c r="I57" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J57" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="13" t="s">
         <v>144</v>
       </c>
@@ -3278,8 +3612,11 @@
       <c r="I58" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J58" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I59" s="3"/>
     </row>
   </sheetData>

</xml_diff>